<commit_message>
ajout d'un fichier similaire Jouer et actu personnes
</commit_message>
<xml_diff>
--- a/cinema_base_saga_personnes.xlsx
+++ b/cinema_base_saga_personnes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="99">
   <si>
     <t xml:space="preserve">nom </t>
   </si>
@@ -39,9 +39,6 @@
     <t>acteur</t>
   </si>
   <si>
-    <t>Dumbledore</t>
-  </si>
-  <si>
     <t>Gambon</t>
   </si>
   <si>
@@ -54,18 +51,12 @@
     <t xml:space="preserve">Maggie </t>
   </si>
   <si>
-    <t>Professor McGonagall</t>
-  </si>
-  <si>
     <t>Coltrane</t>
   </si>
   <si>
     <t>Robbie</t>
   </si>
   <si>
-    <t>Hagrid</t>
-  </si>
-  <si>
     <t>Radcliffe</t>
   </si>
   <si>
@@ -90,9 +81,6 @@
     <t xml:space="preserve">Warwick </t>
   </si>
   <si>
-    <t>SW VIII - VII - VI -  I</t>
-  </si>
-  <si>
     <t>Hurt</t>
   </si>
   <si>
@@ -105,9 +93,6 @@
     <t xml:space="preserve">Domhnall </t>
   </si>
   <si>
-    <t>SW VII - VII - IX</t>
-  </si>
-  <si>
     <t>Columbus</t>
   </si>
   <si>
@@ -135,309 +120,180 @@
     <t xml:space="preserve">David </t>
   </si>
   <si>
-    <t>AF 1-2</t>
-  </si>
-  <si>
     <t>Redmayne</t>
   </si>
   <si>
     <t xml:space="preserve">Eddie </t>
   </si>
   <si>
-    <t>Norbert Dragonneau</t>
-  </si>
-  <si>
     <t>Waterston</t>
   </si>
   <si>
     <t xml:space="preserve">Katherine </t>
   </si>
   <si>
-    <t>Tina Goldstein</t>
-  </si>
-  <si>
     <t>Farrell</t>
   </si>
   <si>
     <t xml:space="preserve">Colin </t>
   </si>
   <si>
-    <t>Percival Graves</t>
-  </si>
-  <si>
     <t>McGregor</t>
   </si>
   <si>
     <t>Ewan</t>
   </si>
   <si>
-    <t>Obi-Wan Kenobi</t>
-  </si>
-  <si>
-    <t>SW VII - III - II- I</t>
-  </si>
-  <si>
     <t>Christensen</t>
   </si>
   <si>
     <t>Hayden</t>
   </si>
   <si>
-    <t>Anakin Skywalker</t>
-  </si>
-  <si>
-    <t>SW II III</t>
-  </si>
-  <si>
     <t>Jones</t>
   </si>
   <si>
     <t>James Earl</t>
   </si>
   <si>
-    <t>Dark Vador (voix)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW IV - V - VI - III </t>
-  </si>
-  <si>
     <t>Daniels</t>
   </si>
   <si>
     <t>Anthony</t>
   </si>
   <si>
-    <t>C3PO</t>
-  </si>
-  <si>
-    <t>SW IV - V - VI - I - II - III - VII - VIII - IX</t>
-  </si>
-  <si>
     <t>Baker</t>
   </si>
   <si>
     <t>Kenny</t>
   </si>
   <si>
-    <t>R2D2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW IV - V - VI - I - II - III </t>
-  </si>
-  <si>
     <t>Mayhew</t>
   </si>
   <si>
     <t>Peter</t>
   </si>
   <si>
-    <t>Chewbacca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SW IV - V - VI -III- VII - </t>
-  </si>
-  <si>
     <t>Hamill</t>
   </si>
   <si>
     <t>Mark</t>
   </si>
   <si>
-    <t>Luke Skywalker</t>
-  </si>
-  <si>
-    <t>SW IV - V - VI - VII - VIII - IX</t>
-  </si>
-  <si>
     <t>Fisher</t>
   </si>
   <si>
     <t>Carrie</t>
   </si>
   <si>
-    <t>Leia Organa</t>
-  </si>
-  <si>
-    <t>SW VII- VIII- IX</t>
-  </si>
-  <si>
     <t>Ford</t>
   </si>
   <si>
     <t>Harrison</t>
   </si>
   <si>
-    <t>Han Solo</t>
-  </si>
-  <si>
-    <t>SW VII</t>
-  </si>
-  <si>
     <t>Lucas</t>
   </si>
   <si>
     <t>Georges</t>
   </si>
   <si>
-    <t>SW I - II - III -  IV</t>
-  </si>
-  <si>
     <t>Kershner</t>
   </si>
   <si>
     <t>Irvin</t>
   </si>
   <si>
-    <t>SW V</t>
-  </si>
-  <si>
     <t>Marquand</t>
   </si>
   <si>
     <t>Richard</t>
   </si>
   <si>
-    <t>SW VI</t>
-  </si>
-  <si>
     <t>Abrams</t>
   </si>
   <si>
     <t>J.J</t>
   </si>
   <si>
-    <t>SW VII - IX</t>
-  </si>
-  <si>
     <t>Johnson</t>
   </si>
   <si>
     <t>Rian</t>
   </si>
   <si>
-    <t>SW VIII</t>
-  </si>
-  <si>
     <t>Holm</t>
   </si>
   <si>
     <t>Ian</t>
   </si>
   <si>
-    <t>Bilbo (vieux)</t>
-  </si>
-  <si>
     <t>Freeman</t>
   </si>
   <si>
     <t>Martin</t>
   </si>
   <si>
-    <t>Bilbo (jeune)</t>
-  </si>
-  <si>
-    <t>H 1-2-3</t>
-  </si>
-  <si>
     <t>Armitage</t>
   </si>
   <si>
-    <t>Thorin</t>
-  </si>
-  <si>
     <t>Weaving</t>
   </si>
   <si>
     <t>Hugo</t>
   </si>
   <si>
-    <t>Elrond</t>
-  </si>
-  <si>
     <t>Bloom</t>
   </si>
   <si>
     <t>Orlando</t>
   </si>
   <si>
-    <t>Legolas</t>
-  </si>
-  <si>
     <t>Blanchett</t>
   </si>
   <si>
     <t>Cate</t>
   </si>
   <si>
-    <t>Galadriel</t>
-  </si>
-  <si>
     <t>Wood</t>
   </si>
   <si>
     <t>Elijah</t>
   </si>
   <si>
-    <t>Frodon</t>
-  </si>
-  <si>
     <t>Lee</t>
   </si>
   <si>
     <t>Christopher</t>
   </si>
   <si>
-    <t>Saroumane</t>
-  </si>
-  <si>
     <t>Serkis</t>
   </si>
   <si>
     <t>Andy</t>
   </si>
   <si>
-    <t>Gollum</t>
-  </si>
-  <si>
-    <t>sw VIII</t>
-  </si>
-  <si>
     <t>McKellen</t>
   </si>
   <si>
-    <t>Gandalf</t>
-  </si>
-  <si>
     <t>Mortensen</t>
   </si>
   <si>
     <t>Viggo</t>
   </si>
   <si>
-    <t>Aragorn</t>
-  </si>
-  <si>
     <t>Bean</t>
   </si>
   <si>
     <t>Sean</t>
   </si>
   <si>
-    <t>Boromir</t>
-  </si>
-  <si>
     <t xml:space="preserve">Astin </t>
   </si>
   <si>
-    <t>Samsagace</t>
-  </si>
-  <si>
     <t>Rhys-Davies</t>
   </si>
   <si>
-    <t>Gimli</t>
-  </si>
-  <si>
     <t>Jackson</t>
   </si>
   <si>
@@ -450,9 +306,6 @@
     <t>compositeur</t>
   </si>
   <si>
-    <t>SW all</t>
-  </si>
-  <si>
     <t>Shore</t>
   </si>
   <si>
@@ -462,97 +315,7 @@
     <t>James Newton</t>
   </si>
   <si>
-    <t>role2</t>
-  </si>
-  <si>
-    <t>roles</t>
-  </si>
-  <si>
-    <t>Wodibin - Wollivan -Wicket -Wald</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Professor Flitwick </t>
-  </si>
-  <si>
-    <t>Harry Potter</t>
-  </si>
-  <si>
-    <t>Hermione Granger</t>
-  </si>
-  <si>
-    <t>Professor Snape</t>
-  </si>
-  <si>
-    <t>Olivander</t>
-  </si>
-  <si>
-    <t xml:space="preserve">narrateur : </t>
-  </si>
-  <si>
-    <t>Dogville</t>
-  </si>
-  <si>
-    <t>film1</t>
-  </si>
-  <si>
-    <t>film2</t>
-  </si>
-  <si>
-    <t>H 1 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOTR 1 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOTR 2 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOTR 1 2 3 </t>
-  </si>
-  <si>
-    <t>Hobbit</t>
-  </si>
-  <si>
-    <t>LOTR</t>
-  </si>
-  <si>
-    <t>HP1-3</t>
-  </si>
-  <si>
-    <t>HP 1 -&gt; 2</t>
-  </si>
-  <si>
-    <t>HP 3 -&gt; 8</t>
-  </si>
-  <si>
-    <t>HP 1 -&gt; 8</t>
-  </si>
-  <si>
-    <t>HP 1 -7 - 8</t>
-  </si>
-  <si>
-    <t>HP 7 -&gt; 8</t>
-  </si>
-  <si>
-    <t>HP 3</t>
-  </si>
-  <si>
-    <t>HP 4</t>
-  </si>
-  <si>
-    <t>HP 5 -&gt; 8</t>
-  </si>
-  <si>
-    <t>LOTR 1 2 (3 )</t>
-  </si>
-  <si>
-    <t>LOTR 1 (2 3 )</t>
-  </si>
-  <si>
-    <t>Général Hux</t>
-  </si>
-  <si>
-    <t>Bill Weasley</t>
+    <t>fonctionFilm</t>
   </si>
 </sst>
 </file>
@@ -1360,15 +1123,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1378,20 +1141,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G1" t="s">
-        <v>157</v>
-      </c>
-      <c r="H1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1404,19 +1158,13 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
       <c r="C4" s="1">
         <v>14903</v>
@@ -1424,19 +1172,13 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
       </c>
       <c r="C5" s="1">
         <v>12781</v>
@@ -1444,19 +1186,13 @@
       <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
-      </c>
-      <c r="G5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
       </c>
       <c r="C6" s="1">
         <v>18352</v>
@@ -1464,19 +1200,13 @@
       <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1">
         <v>32712</v>
@@ -1484,19 +1214,13 @@
       <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" t="s">
-        <v>151</v>
-      </c>
-      <c r="G7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1">
         <v>32978</v>
@@ -1504,19 +1228,13 @@
       <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" t="s">
-        <v>152</v>
-      </c>
-      <c r="G8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1">
         <v>16854</v>
@@ -1524,19 +1242,13 @@
       <c r="D9" t="s">
         <v>5</v>
       </c>
-      <c r="E9" t="s">
-        <v>153</v>
-      </c>
-      <c r="G9" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1">
         <v>25602</v>
@@ -1544,25 +1256,13 @@
       <c r="D10" t="s">
         <v>5</v>
       </c>
-      <c r="E10" t="s">
-        <v>150</v>
-      </c>
-      <c r="F10" t="s">
-        <v>149</v>
-      </c>
-      <c r="G10" t="s">
-        <v>168</v>
-      </c>
-      <c r="H10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1">
         <v>14632</v>
@@ -1570,25 +1270,13 @@
       <c r="D11" t="s">
         <v>5</v>
       </c>
-      <c r="E11" t="s">
-        <v>154</v>
-      </c>
-      <c r="F11" t="s">
-        <v>155</v>
-      </c>
-      <c r="G11" t="s">
-        <v>169</v>
-      </c>
-      <c r="H11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1">
         <v>30448</v>
@@ -1596,96 +1284,69 @@
       <c r="D12" t="s">
         <v>5</v>
       </c>
-      <c r="E12" t="s">
-        <v>177</v>
-      </c>
-      <c r="F12" t="s">
-        <v>176</v>
-      </c>
-      <c r="G12" t="s">
-        <v>170</v>
-      </c>
-      <c r="H12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1">
         <v>21438</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1">
         <v>22613</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1">
         <v>15428</v>
       </c>
       <c r="D16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="G16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1">
         <v>23292</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" t="s">
-        <v>173</v>
-      </c>
-      <c r="H17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C19" s="1">
         <v>29957</v>
@@ -1693,19 +1354,13 @@
       <c r="D19" t="s">
         <v>5</v>
       </c>
-      <c r="E19" t="s">
-        <v>41</v>
-      </c>
-      <c r="G19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1">
         <v>29283</v>
@@ -1713,19 +1368,13 @@
       <c r="D20" t="s">
         <v>5</v>
       </c>
-      <c r="E20" t="s">
-        <v>44</v>
-      </c>
-      <c r="G20" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" t="s">
-        <v>46</v>
       </c>
       <c r="C21" s="1">
         <v>27911</v>
@@ -1733,19 +1382,13 @@
       <c r="D21" t="s">
         <v>5</v>
       </c>
-      <c r="E21" t="s">
-        <v>47</v>
-      </c>
-      <c r="G21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C24" s="1">
         <v>26023</v>
@@ -1753,19 +1396,13 @@
       <c r="D24" t="s">
         <v>5</v>
       </c>
-      <c r="E24" t="s">
-        <v>50</v>
-      </c>
-      <c r="G24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C25" s="1">
         <v>29725</v>
@@ -1773,19 +1410,13 @@
       <c r="D25" t="s">
         <v>5</v>
       </c>
-      <c r="E25" t="s">
-        <v>54</v>
-      </c>
-      <c r="G25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="C26" s="1">
         <v>11340</v>
@@ -1793,19 +1424,13 @@
       <c r="D26" t="s">
         <v>5</v>
       </c>
-      <c r="E26" t="s">
-        <v>58</v>
-      </c>
-      <c r="G26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C27" s="1">
         <v>32054</v>
@@ -1813,19 +1438,13 @@
       <c r="D27" t="s">
         <v>5</v>
       </c>
-      <c r="E27" t="s">
-        <v>62</v>
-      </c>
-      <c r="G27" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C28" s="1">
         <v>12655</v>
@@ -1833,19 +1452,13 @@
       <c r="D28" t="s">
         <v>5</v>
       </c>
-      <c r="E28" t="s">
-        <v>66</v>
-      </c>
-      <c r="G28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="C29" s="1">
         <v>16211</v>
@@ -1853,19 +1466,13 @@
       <c r="D29" t="s">
         <v>5</v>
       </c>
-      <c r="E29" t="s">
-        <v>70</v>
-      </c>
-      <c r="G29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="C30" s="1">
         <v>18896</v>
@@ -1873,19 +1480,13 @@
       <c r="D30" t="s">
         <v>5</v>
       </c>
-      <c r="E30" t="s">
-        <v>74</v>
-      </c>
-      <c r="G30" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="C31" s="1">
         <v>20816</v>
@@ -1893,19 +1494,13 @@
       <c r="D31" t="s">
         <v>5</v>
       </c>
-      <c r="E31" t="s">
-        <v>78</v>
-      </c>
-      <c r="G31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="C32" s="1">
         <v>15535</v>
@@ -1913,104 +1508,83 @@
       <c r="D32" t="s">
         <v>5</v>
       </c>
-      <c r="E32" t="s">
-        <v>82</v>
-      </c>
-      <c r="G32" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="C33" s="1">
         <v>16206</v>
       </c>
       <c r="D33" t="s">
-        <v>31</v>
-      </c>
-      <c r="G33" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="C34" s="1">
         <v>8520</v>
       </c>
       <c r="D34" t="s">
-        <v>31</v>
-      </c>
-      <c r="G34" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="C35" s="1">
         <v>13780</v>
       </c>
       <c r="D35" t="s">
-        <v>31</v>
-      </c>
-      <c r="G35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="C36" s="1">
         <v>24285</v>
       </c>
       <c r="D36" t="s">
-        <v>31</v>
-      </c>
-      <c r="G36" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="C37" s="1">
         <v>27015</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
-      </c>
-      <c r="G37" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="B39" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="C39" s="1">
         <v>11578</v>
@@ -2018,22 +1592,13 @@
       <c r="D39" t="s">
         <v>5</v>
       </c>
-      <c r="E39" t="s">
-        <v>101</v>
-      </c>
-      <c r="G39" t="s">
-        <v>159</v>
-      </c>
-      <c r="H39" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="C40" s="1">
         <v>26184</v>
@@ -2041,19 +1606,13 @@
       <c r="D40" t="s">
         <v>5</v>
       </c>
-      <c r="E40" t="s">
-        <v>104</v>
-      </c>
-      <c r="G40" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="B41" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="C41" s="1">
         <v>26167</v>
@@ -2061,19 +1620,13 @@
       <c r="D41" t="s">
         <v>5</v>
       </c>
-      <c r="E41" t="s">
-        <v>107</v>
-      </c>
-      <c r="G41" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="B42" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="C42" s="1">
         <v>22010</v>
@@ -2081,22 +1634,13 @@
       <c r="D42" t="s">
         <v>5</v>
       </c>
-      <c r="E42" t="s">
-        <v>110</v>
-      </c>
-      <c r="G42" t="s">
-        <v>105</v>
-      </c>
-      <c r="H42" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>74</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>75</v>
       </c>
       <c r="C43" s="1">
         <v>28138</v>
@@ -2104,22 +1648,13 @@
       <c r="D43" t="s">
         <v>5</v>
       </c>
-      <c r="E43" t="s">
-        <v>113</v>
-      </c>
-      <c r="G43" t="s">
-        <v>105</v>
-      </c>
-      <c r="H43" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="B44" t="s">
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="C44" s="1">
         <v>25337</v>
@@ -2127,22 +1662,13 @@
       <c r="D44" t="s">
         <v>5</v>
       </c>
-      <c r="E44" t="s">
-        <v>116</v>
-      </c>
-      <c r="G44" t="s">
-        <v>105</v>
-      </c>
-      <c r="H44" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>117</v>
+        <v>78</v>
       </c>
       <c r="B45" t="s">
-        <v>118</v>
+        <v>79</v>
       </c>
       <c r="C45" s="1">
         <v>29614</v>
@@ -2150,19 +1676,13 @@
       <c r="D45" t="s">
         <v>5</v>
       </c>
-      <c r="E45" t="s">
-        <v>119</v>
-      </c>
-      <c r="G45" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="C46" s="1">
         <v>8183</v>
@@ -2170,19 +1690,13 @@
       <c r="D46" t="s">
         <v>5</v>
       </c>
-      <c r="E46" t="s">
-        <v>122</v>
-      </c>
-      <c r="G46" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
       <c r="B47" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="C47" s="1">
         <v>23487</v>
@@ -2190,22 +1704,13 @@
       <c r="D47" t="s">
         <v>5</v>
       </c>
-      <c r="E47" t="s">
-        <v>125</v>
-      </c>
-      <c r="G47" t="s">
-        <v>162</v>
-      </c>
-      <c r="H47" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="C48" s="1">
         <v>14390</v>
@@ -2213,19 +1718,13 @@
       <c r="D48" t="s">
         <v>5</v>
       </c>
-      <c r="E48" t="s">
-        <v>128</v>
-      </c>
-      <c r="G48" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="B49" t="s">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="C49" s="1">
         <v>21478</v>
@@ -2233,19 +1732,13 @@
       <c r="D49" t="s">
         <v>5</v>
       </c>
-      <c r="E49" t="s">
-        <v>131</v>
-      </c>
-      <c r="G49" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>132</v>
+        <v>87</v>
       </c>
       <c r="B50" t="s">
-        <v>133</v>
+        <v>88</v>
       </c>
       <c r="C50" s="1">
         <v>21657</v>
@@ -2253,19 +1746,13 @@
       <c r="D50" t="s">
         <v>5</v>
       </c>
-      <c r="E50" t="s">
-        <v>134</v>
-      </c>
-      <c r="G50" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="B51" t="s">
-        <v>133</v>
+        <v>88</v>
       </c>
       <c r="C51" s="1">
         <v>25989</v>
@@ -2273,19 +1760,13 @@
       <c r="D51" t="s">
         <v>5</v>
       </c>
-      <c r="E51" t="s">
-        <v>136</v>
-      </c>
-      <c r="G51" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>137</v>
+        <v>90</v>
       </c>
       <c r="B52" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C52" s="1">
         <v>16197</v>
@@ -2293,88 +1774,61 @@
       <c r="D52" t="s">
         <v>5</v>
       </c>
-      <c r="E52" t="s">
-        <v>138</v>
-      </c>
-      <c r="G52" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>139</v>
+        <v>91</v>
       </c>
       <c r="B54" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="C54" s="1">
         <v>22585</v>
       </c>
       <c r="D54" t="s">
-        <v>31</v>
-      </c>
-      <c r="G54" t="s">
-        <v>164</v>
-      </c>
-      <c r="H54" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>140</v>
+        <v>92</v>
       </c>
       <c r="B56" t="s">
-        <v>141</v>
+        <v>93</v>
       </c>
       <c r="C56" s="1">
         <v>11727</v>
       </c>
       <c r="D56" t="s">
-        <v>142</v>
-      </c>
-      <c r="G56" t="s">
-        <v>165</v>
-      </c>
-      <c r="H56" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>144</v>
+        <v>95</v>
       </c>
       <c r="B57" t="s">
-        <v>145</v>
+        <v>96</v>
       </c>
       <c r="C57" s="1">
         <v>17093</v>
       </c>
       <c r="D57" t="s">
-        <v>142</v>
-      </c>
-      <c r="G57" t="s">
-        <v>164</v>
-      </c>
-      <c r="H57" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>145</v>
+        <v>96</v>
       </c>
       <c r="B58" t="s">
-        <v>146</v>
+        <v>97</v>
       </c>
       <c r="C58" s="1">
         <v>18788</v>
       </c>
       <c r="D58" t="s">
-        <v>142</v>
-      </c>
-      <c r="G58" t="s">
-        <v>38</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>